<commit_message>
Change Servo M0 linear equation
</commit_message>
<xml_diff>
--- a/Servo.xlsx
+++ b/Servo.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18220" windowHeight="16720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HS-422" sheetId="1" r:id="rId1"/>
-    <sheet name="M1" sheetId="2" r:id="rId2"/>
+    <sheet name="M0" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -22,6 +22,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,8 +59,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -232,11 +239,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2093134976"/>
-        <c:axId val="-2093125312"/>
+        <c:axId val="-2130807008"/>
+        <c:axId val="-2130803168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2093134976"/>
+        <c:axId val="-2130807008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -292,12 +299,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093125312"/>
+        <c:crossAx val="-2130803168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2093125312"/>
+        <c:axId val="-2130803168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -354,7 +361,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2093134976"/>
+        <c:crossAx val="-2130807008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -495,8 +502,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.103794181977253"/>
-                  <c:y val="-0.000416666666666667"/>
+                  <c:x val="-0.159349737532808"/>
+                  <c:y val="0.0540327496293844"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -531,17 +538,14 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'M1'!$A$1:$A$3</c:f>
+              <c:f>M0!$A$1:$A$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>180.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -549,18 +553,15 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'M1'!$B$1:$B$3</c:f>
+              <c:f>M0!$B$1:$B$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>625000.0</c:v>
+                  <c:v>509167.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.45E6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.25E6</c:v>
+                  <c:v>2.304027E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,11 +576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2084997600"/>
-        <c:axId val="-2054455040"/>
+        <c:axId val="-2103390512"/>
+        <c:axId val="-2103387168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2084997600"/>
+        <c:axId val="-2103390512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,12 +637,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054455040"/>
+        <c:crossAx val="-2103387168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2054455040"/>
+        <c:axId val="-2103387168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,7 +699,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084997600"/>
+        <c:crossAx val="-2103390512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1900,13 +1901,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2194,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="64" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -2253,37 +2254,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>625000</v>
+        <v>509167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="B2">
-        <v>1450000</v>
+        <v>2304027</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>180</v>
-      </c>
-      <c r="B3">
-        <v>2250000</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>